<commit_message>
push test case registrasi 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C5D37-E460-4AFC-9AF2-BA364802FED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F42588C-3A4F-4E77-924C-CB259820DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>REG-02</t>
   </si>
   <si>
     <t>Medium</t>
@@ -270,6 +273,26 @@
   </si>
   <si>
     <t>Registration Successful</t>
+  </si>
+  <si>
+    <t>REG-TC-02</t>
+  </si>
+  <si>
+    <t>Register using already registered email</t>
+  </si>
+  <si>
+    <t>Email already exists</t>
+  </si>
+  <si>
+    <t>1. Input existing email 
+2. Input valid password 
+3. Click register</t>
+  </si>
+  <si>
+    <t>Error message appears</t>
+  </si>
+  <si>
+    <t>user1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -695,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
-  <dimension ref="B3:L4"/>
+  <dimension ref="B3:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,88 +730,113 @@
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="I4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="K4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{A23E3B46-2CB3-4E84-AECF-8CB3118A96C2}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{A23E3B46-2CB3-4E84-AECF-8CB3118A96C2}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{588198C3-2C33-47E3-8C8E-545667B2835C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -830,16 +878,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -847,16 +895,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -864,16 +912,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -881,16 +929,16 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
@@ -898,16 +946,16 @@
     </row>
     <row r="8" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
@@ -955,16 +1003,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -972,16 +1020,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -989,16 +1037,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1046,16 +1094,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1063,16 +1111,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1080,16 +1128,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1137,16 +1185,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1154,16 +1202,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1171,16 +1219,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1228,33 +1276,33 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1262,16 +1310,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
push test case registrasi 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F42588C-3A4F-4E77-924C-CB259820DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB9461F-F8B2-4565-8A2A-6AAF0D03E176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>REG-02</t>
+  </si>
+  <si>
+    <t>REG-03</t>
   </si>
   <si>
     <t>Medium</t>
@@ -278,10 +281,10 @@
     <t>REG-TC-02</t>
   </si>
   <si>
+    <t>REG-TC-03</t>
+  </si>
+  <si>
     <t>Register using already registered email</t>
-  </si>
-  <si>
-    <t>Email already exists</t>
   </si>
   <si>
     <t>1. Input existing email 
@@ -293,6 +296,24 @@
   </si>
   <si>
     <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>Register with invalid email format</t>
+  </si>
+  <si>
+    <t>On registration page</t>
+  </si>
+  <si>
+    <t>On registration page and 
+email already exists</t>
+  </si>
+  <si>
+    <t>1. Input invalid email 
+2. Input password 
+3. Click register</t>
+  </si>
+  <si>
+    <t>usermail.com</t>
   </si>
 </sst>
 </file>
@@ -718,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
-  <dimension ref="B3:K5"/>
+  <dimension ref="B3:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,31 +759,31 @@
   <sheetData>
     <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>4</v>
@@ -773,28 +794,28 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>6</v>
@@ -805,31 +826,63 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>6</v>
+      <c r="K6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -837,6 +890,7 @@
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{A23E3B46-2CB3-4E84-AECF-8CB3118A96C2}"/>
     <hyperlink ref="I5" r:id="rId2" xr:uid="{588198C3-2C33-47E3-8C8E-545667B2835C}"/>
+    <hyperlink ref="I6" r:id="rId3" display="user1@gmail.com" xr:uid="{D32F4EEB-7483-4369-B4DE-A4D9600F4CC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -878,16 +932,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -895,16 +949,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -912,16 +966,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -929,16 +983,16 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
@@ -946,16 +1000,16 @@
     </row>
     <row r="8" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
@@ -1003,16 +1057,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1020,16 +1074,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1037,16 +1091,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1094,16 +1148,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1111,16 +1165,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1128,16 +1182,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1185,16 +1239,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1202,16 +1256,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1219,16 +1273,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1276,33 +1330,33 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1310,16 +1364,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
push test case registrasi 4
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB9461F-F8B2-4565-8A2A-6AAF0D03E176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D275FFA-75E5-4BF0-A979-2EF513B42CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -53,10 +53,19 @@
     <t>High</t>
   </si>
   <si>
+    <t>Verify user can register with valid email and password</t>
+  </si>
+  <si>
+    <t>Verify system prevents duplicate email registration</t>
+  </si>
+  <si>
     <t>REG-02</t>
   </si>
   <si>
     <t>REG-03</t>
+  </si>
+  <si>
+    <t>REG-04</t>
   </si>
   <si>
     <t>Medium</t>
@@ -284,6 +293,12 @@
     <t>REG-TC-03</t>
   </si>
   <si>
+    <t>REG-TC-04</t>
+  </si>
+  <si>
+    <t>REG-TC-05</t>
+  </si>
+  <si>
     <t>Register using already registered email</t>
   </si>
   <si>
@@ -314,6 +329,37 @@
   </si>
   <si>
     <t>usermail.com</t>
+  </si>
+  <si>
+    <t>Register with password less than 8 characters</t>
+  </si>
+  <si>
+    <t>1. Input valid email 
+2. Input short password 
+3. Click register</t>
+  </si>
+  <si>
+    <t>Pass12</t>
+  </si>
+  <si>
+    <t>Register with exactly 8 characters password</t>
+  </si>
+  <si>
+    <t>1. Input valid email 
+2. Input 8-character password 
+3. Click register</t>
+  </si>
+  <si>
+    <t>Pass1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario </t>
+  </si>
+  <si>
+    <t>Verify system validates email format</t>
+  </si>
+  <si>
+    <t>Verify minimum password length (8 characters)</t>
   </si>
 </sst>
 </file>
@@ -356,7 +402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,8 +421,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -399,12 +451,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,6 +500,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,158 +832,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
-  <dimension ref="B3:K6"/>
+  <dimension ref="B3:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
+      <c r="C4" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="63" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>9</v>
+      <c r="L8" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{A23E3B46-2CB3-4E84-AECF-8CB3118A96C2}"/>
-    <hyperlink ref="I5" r:id="rId2" xr:uid="{588198C3-2C33-47E3-8C8E-545667B2835C}"/>
-    <hyperlink ref="I6" r:id="rId3" display="user1@gmail.com" xr:uid="{D32F4EEB-7483-4369-B4DE-A4D9600F4CC2}"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{A23E3B46-2CB3-4E84-AECF-8CB3118A96C2}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{588198C3-2C33-47E3-8C8E-545667B2835C}"/>
+    <hyperlink ref="J6" r:id="rId3" display="user1@gmail.com" xr:uid="{D32F4EEB-7483-4369-B4DE-A4D9600F4CC2}"/>
+    <hyperlink ref="J7" r:id="rId4" display="user1@gmail.com" xr:uid="{310A0BA6-3448-4D02-95A4-24659727C4F2}"/>
+    <hyperlink ref="J8" r:id="rId5" display="user1@gmail.com" xr:uid="{C1EA0C6B-08AA-4073-B54F-F79EFCDF8FAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -932,16 +1111,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -949,16 +1128,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -966,16 +1145,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -983,16 +1162,16 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
@@ -1000,16 +1179,16 @@
     </row>
     <row r="8" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
@@ -1057,16 +1236,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1074,16 +1253,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1091,16 +1270,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1148,16 +1327,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1165,16 +1344,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1182,16 +1361,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1239,16 +1418,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1256,16 +1435,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1273,16 +1452,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1330,33 +1509,33 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1364,16 +1543,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
push test case registrasi 5
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D275FFA-75E5-4BF0-A979-2EF513B42CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4361429-C108-49FD-A523-7A60E8CC0CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>REG-04</t>
+  </si>
+  <si>
+    <t>REG-05</t>
   </si>
   <si>
     <t>Medium</t>
@@ -299,6 +302,9 @@
     <t>REG-TC-05</t>
   </si>
   <si>
+    <t>REG-TC-06</t>
+  </si>
+  <si>
     <t>Register using already registered email</t>
   </si>
   <si>
@@ -360,6 +366,31 @@
   </si>
   <si>
     <t>Verify minimum password length (8 characters)</t>
+  </si>
+  <si>
+    <t>REG-TC-07</t>
+  </si>
+  <si>
+    <t>Verify required fields cannot be empty</t>
+  </si>
+  <si>
+    <t>Register with empty email</t>
+  </si>
+  <si>
+    <t>Leave email empty, fill password, click register</t>
+  </si>
+  <si>
+    <t>"" / Password123</t>
+  </si>
+  <si>
+    <t>Fill email, leave password empty, click register</t>
+  </si>
+  <si>
+    <t>user2@mail.com
+ / ""</t>
+  </si>
+  <si>
+    <t>Fill email, leave password empty, click registe</t>
   </si>
 </sst>
 </file>
@@ -832,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
-  <dimension ref="B3:L8"/>
+  <dimension ref="B3:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,34 +885,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>4</v>
@@ -895,28 +926,28 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>6</v>
@@ -930,28 +961,28 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>6</v>
@@ -962,34 +993,34 @@
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -997,31 +1028,31 @@
         <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>6</v>
@@ -1031,37 +1062,105 @@
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
       <c r="D8" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1070,6 +1169,8 @@
     <hyperlink ref="J6" r:id="rId3" display="user1@gmail.com" xr:uid="{D32F4EEB-7483-4369-B4DE-A4D9600F4CC2}"/>
     <hyperlink ref="J7" r:id="rId4" display="user1@gmail.com" xr:uid="{310A0BA6-3448-4D02-95A4-24659727C4F2}"/>
     <hyperlink ref="J8" r:id="rId5" display="user1@gmail.com" xr:uid="{C1EA0C6B-08AA-4073-B54F-F79EFCDF8FAF}"/>
+    <hyperlink ref="J9" r:id="rId6" display="user1@gmail.com" xr:uid="{D2DF9552-17F4-4571-AD6D-B4F692D356F4}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{07DA7638-2EC3-4717-A6F0-4EE17B606C64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1111,16 +1212,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1128,16 +1229,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1145,16 +1246,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1162,16 +1263,16 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
@@ -1179,16 +1280,16 @@
     </row>
     <row r="8" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
@@ -1236,16 +1337,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1253,16 +1354,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1270,16 +1371,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1327,16 +1428,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1344,16 +1445,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1361,16 +1462,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1418,16 +1519,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1435,16 +1536,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1452,16 +1553,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1509,33 +1610,33 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1543,16 +1644,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
push test case registrasi 6
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4361429-C108-49FD-A523-7A60E8CC0CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153A9C79-C2AA-4AE3-B1F9-97A853416290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="124">
   <si>
     <t>Scenario ID</t>
   </si>
@@ -71,7 +71,13 @@
     <t>REG-05</t>
   </si>
   <si>
+    <t>REG-06</t>
+  </si>
+  <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Verify user can login after successful registration</t>
   </si>
   <si>
     <t>Registration Module</t>
@@ -391,6 +397,27 @@
   </si>
   <si>
     <t>Fill email, leave password empty, click registe</t>
+  </si>
+  <si>
+    <t>REG-TC-08</t>
+  </si>
+  <si>
+    <t>Login after successful registration</t>
+  </si>
+  <si>
+    <t>User already registered</t>
+  </si>
+  <si>
+    <t>1. Go to login page 
+2. Input registered email &amp; password 
+3. Click login</t>
+  </si>
+  <si>
+    <t>user1@mail.com
+ / Password123</t>
+  </si>
+  <si>
+    <t>User successfully logged in</t>
   </si>
 </sst>
 </file>
@@ -863,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
-  <dimension ref="B3:L10"/>
+  <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,34 +912,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>4</v>
@@ -926,28 +953,28 @@
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>6</v>
@@ -961,28 +988,28 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>6</v>
@@ -993,34 +1020,34 @@
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1028,31 +1055,31 @@
         <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>6</v>
@@ -1062,28 +1089,28 @@
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>6</v>
@@ -1094,31 +1121,31 @@
         <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>6</v>
@@ -1128,33 +1155,69 @@
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="2:12" ht="63" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B7:B8"/>
@@ -1171,6 +1234,7 @@
     <hyperlink ref="J8" r:id="rId5" display="user1@gmail.com" xr:uid="{C1EA0C6B-08AA-4073-B54F-F79EFCDF8FAF}"/>
     <hyperlink ref="J9" r:id="rId6" display="user1@gmail.com" xr:uid="{D2DF9552-17F4-4571-AD6D-B4F692D356F4}"/>
     <hyperlink ref="J10" r:id="rId7" xr:uid="{07DA7638-2EC3-4717-A6F0-4EE17B606C64}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{3F4FE4F2-9EB5-4B7D-BC78-9A44486C111D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1212,16 +1276,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1229,16 +1293,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1246,16 +1310,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1263,16 +1327,16 @@
     </row>
     <row r="7" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>6</v>
@@ -1280,16 +1344,16 @@
     </row>
     <row r="8" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>6</v>
@@ -1337,16 +1401,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1354,16 +1418,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1371,16 +1435,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1428,16 +1492,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1445,16 +1509,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1462,16 +1526,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1519,16 +1583,16 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -1536,16 +1600,16 @@
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1553,16 +1617,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>
@@ -1610,33 +1674,33 @@
     </row>
     <row r="4" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -1644,16 +1708,16 @@
     </row>
     <row r="6" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
upload test case login 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566707F5-A0B3-491E-BD4F-7C35323F866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06414C-A11B-4F51-88B0-C618BE68550B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>Module</t>
   </si>
@@ -76,7 +76,13 @@
     <t>LOG-01</t>
   </si>
   <si>
+    <t>LOG-02</t>
+  </si>
+  <si>
     <t>LOG-TS-01</t>
+  </si>
+  <si>
+    <t>LOG-TS-02</t>
   </si>
   <si>
     <t>Verify user can login with valid email and password</t>
@@ -264,6 +270,31 @@
 2. Enter valid email 
 3. Enter valid password 
 4. Click Login</t>
+  </si>
+  <si>
+    <t>LOG-TC-02</t>
+  </si>
+  <si>
+    <t>Verify system displays error when password is incorrect</t>
+  </si>
+  <si>
+    <t>Login with incorrect password</t>
+  </si>
+  <si>
+    <t>Email already registered</t>
+  </si>
+  <si>
+    <t>1. Open login page 
+2. Enter registered email 
+3. Enter wrong password 
+4. Click Login</t>
+  </si>
+  <si>
+    <t>user1@gmail.com
+WrongPass</t>
+  </si>
+  <si>
+    <t>Error message displayed</t>
   </si>
 </sst>
 </file>
@@ -755,34 +786,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -796,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -805,19 +836,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -831,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -840,19 +871,19 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -863,10 +894,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -875,19 +906,19 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -898,10 +929,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -910,19 +941,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
@@ -932,7 +963,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -941,19 +972,19 @@
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
@@ -964,10 +995,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -976,19 +1007,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>3</v>
@@ -998,7 +1029,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1007,19 +1038,19 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>3</v>
@@ -1033,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -1042,19 +1073,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>3</v>
@@ -1087,14 +1118,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -1108,34 +1139,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -1146,33 +1177,68 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="C5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1181,6 +1247,7 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{A26063F8-C4DF-4248-8592-A7082F19948A}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{1333E85D-EF6C-4F26-BC56-F51F81429501}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload test case login 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06414C-A11B-4F51-88B0-C618BE68550B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEEA6F2-B09A-4DE7-95B5-8E6B686E6055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
   <si>
     <t>Module</t>
   </si>
@@ -79,10 +79,16 @@
     <t>LOG-02</t>
   </si>
   <si>
+    <t>LOG-03</t>
+  </si>
+  <si>
     <t>LOG-TS-01</t>
   </si>
   <si>
     <t>LOG-TS-02</t>
+  </si>
+  <si>
+    <t>LOG-TS-03</t>
   </si>
   <si>
     <t>Verify user can login with valid email and password</t>
@@ -295,6 +301,27 @@
   </si>
   <si>
     <t>Error message displayed</t>
+  </si>
+  <si>
+    <t>LOG-TC-03</t>
+  </si>
+  <si>
+    <t>Verify error when email not registered</t>
+  </si>
+  <si>
+    <t>Login with unregistered email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On login page </t>
+  </si>
+  <si>
+    <t>1. Enter unregistered email 
+2. Enter any password 
+3. Click Login</t>
+  </si>
+  <si>
+    <t>unkown@gmail.com
+Password123</t>
   </si>
 </sst>
 </file>
@@ -786,34 +813,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -827,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -836,19 +863,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -862,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -871,19 +898,19 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -894,10 +921,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -906,19 +933,19 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -929,10 +956,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -941,19 +968,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
@@ -963,7 +990,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -972,19 +999,19 @@
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
@@ -995,10 +1022,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -1007,19 +1034,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>3</v>
@@ -1029,7 +1056,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1038,19 +1065,19 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>3</v>
@@ -1064,7 +1091,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -1073,19 +1100,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>3</v>
@@ -1118,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,34 +1166,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -1177,31 +1204,31 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -1212,33 +1239,68 @@
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="63" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1248,6 +1310,7 @@
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{A26063F8-C4DF-4248-8592-A7082F19948A}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{1333E85D-EF6C-4F26-BC56-F51F81429501}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{7EEBE029-AB84-4539-9F15-5BF65D69E36D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload test case login 4 #1
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEEA6F2-B09A-4DE7-95B5-8E6B686E6055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914739AE-A91F-403B-8D5E-5C840F022BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>Module</t>
   </si>
@@ -82,6 +82,9 @@
     <t>LOG-03</t>
   </si>
   <si>
+    <t>LOG-04</t>
+  </si>
+  <si>
     <t>LOG-TS-01</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t>LOG-TS-03</t>
+  </si>
+  <si>
+    <t>LOG-TS-04</t>
   </si>
   <si>
     <t>Verify user can login with valid email and password</t>
@@ -322,6 +328,25 @@
   <si>
     <t>unkown@gmail.com
 Password123</t>
+  </si>
+  <si>
+    <t>LOG-TC-04</t>
+  </si>
+  <si>
+    <t>Verify required fields validation</t>
+  </si>
+  <si>
+    <t>Login with empty email</t>
+  </si>
+  <si>
+    <t>Leave email empty, enter password, click Login</t>
+  </si>
+  <si>
+    <t>""
+Password124</t>
+  </si>
+  <si>
+    <t>Validation message appears</t>
   </si>
 </sst>
 </file>
@@ -813,34 +838,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -854,7 +879,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -863,19 +888,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -889,7 +914,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -898,19 +923,19 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -921,10 +946,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -933,19 +958,19 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -956,10 +981,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -968,19 +993,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
@@ -990,7 +1015,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -999,19 +1024,19 @@
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
@@ -1022,10 +1047,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -1034,19 +1059,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>3</v>
@@ -1056,7 +1081,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1065,19 +1090,19 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>3</v>
@@ -1091,7 +1116,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -1100,19 +1125,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>3</v>
@@ -1145,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,40 +1185,40 @@
     <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -1204,31 +1229,31 @@
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -1239,31 +1264,31 @@
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -1274,33 +1299,68 @@
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="I7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1311,6 +1371,7 @@
     <hyperlink ref="J4" r:id="rId1" xr:uid="{A26063F8-C4DF-4248-8592-A7082F19948A}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{1333E85D-EF6C-4F26-BC56-F51F81429501}"/>
     <hyperlink ref="J6" r:id="rId3" xr:uid="{7EEBE029-AB84-4539-9F15-5BF65D69E36D}"/>
+    <hyperlink ref="J7" r:id="rId4" display="unkown@gmail.com_x000a_Password123" xr:uid="{8E9299D3-48E0-4C38-B73F-1B32DD1DAF75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload test case login 4 #2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914739AE-A91F-403B-8D5E-5C840F022BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E37D89-B6E6-4739-8C04-79453AD62C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
   <si>
     <t>Module</t>
   </si>
@@ -347,6 +347,19 @@
   </si>
   <si>
     <t>Validation message appears</t>
+  </si>
+  <si>
+    <t>LOG-TC-05</t>
+  </si>
+  <si>
+    <t>Login with empty password</t>
+  </si>
+  <si>
+    <t>Enter email, leave password empty, click Login</t>
+  </si>
+  <si>
+    <t>user1@gmail.com
+""</t>
   </si>
 </sst>
 </file>
@@ -1170,15 +1183,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
@@ -1330,10 +1343,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1361,17 +1374,53 @@
         <v>97</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{A26063F8-C4DF-4248-8592-A7082F19948A}"/>
     <hyperlink ref="J5" r:id="rId2" xr:uid="{1333E85D-EF6C-4F26-BC56-F51F81429501}"/>
     <hyperlink ref="J6" r:id="rId3" xr:uid="{7EEBE029-AB84-4539-9F15-5BF65D69E36D}"/>
     <hyperlink ref="J7" r:id="rId4" display="unkown@gmail.com_x000a_Password123" xr:uid="{8E9299D3-48E0-4C38-B73F-1B32DD1DAF75}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{06B734FC-2BFE-49EA-8A3D-643EA76C66E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload test case login 4 #3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E37D89-B6E6-4739-8C04-79453AD62C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7064C43A-333E-4A3C-8975-0D882C286FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>Module</t>
   </si>
@@ -359,6 +359,19 @@
   </si>
   <si>
     <t>user1@gmail.com
+""</t>
+  </si>
+  <si>
+    <t>LOG-TC-06</t>
+  </si>
+  <si>
+    <t>Login with both fields empty</t>
+  </si>
+  <si>
+    <t>Leave both fields empty, click Login</t>
+  </si>
+  <si>
+    <t>""
 ""</t>
   </si>
 </sst>
@@ -482,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,6 +525,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1183,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,10 +1362,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="12" t="s">
         <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1378,8 +1397,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
         <v>98</v>
       </c>
@@ -1408,11 +1427,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -1421,6 +1472,7 @@
     <hyperlink ref="J6" r:id="rId3" xr:uid="{7EEBE029-AB84-4539-9F15-5BF65D69E36D}"/>
     <hyperlink ref="J7" r:id="rId4" display="unkown@gmail.com_x000a_Password123" xr:uid="{8E9299D3-48E0-4C38-B73F-1B32DD1DAF75}"/>
     <hyperlink ref="J8" r:id="rId5" xr:uid="{06B734FC-2BFE-49EA-8A3D-643EA76C66E3}"/>
+    <hyperlink ref="J9" r:id="rId6" display="user1@gmail.com_x000a_&quot;&quot;" xr:uid="{80DFB4DC-83B4-45F7-BB88-3569EF28A690}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload test case login 5
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7064C43A-333E-4A3C-8975-0D882C286FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E32681-AC2C-41A4-9DED-DFD02B2D774F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="112">
   <si>
     <t>Module</t>
   </si>
@@ -85,6 +85,9 @@
     <t>LOG-04</t>
   </si>
   <si>
+    <t>LOG-05</t>
+  </si>
+  <si>
     <t>LOG-TS-01</t>
   </si>
   <si>
@@ -97,7 +100,13 @@
     <t>LOG-TS-04</t>
   </si>
   <si>
+    <t>LOG-TS-05</t>
+  </si>
+  <si>
     <t>Verify user can login with valid email and password</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to dashboard after successful login</t>
   </si>
   <si>
     <t>TC ID</t>
@@ -365,6 +374,9 @@
     <t>LOG-TC-06</t>
   </si>
   <si>
+    <t>LOG-TC-07</t>
+  </si>
+  <si>
     <t>Login with both fields empty</t>
   </si>
   <si>
@@ -373,6 +385,13 @@
   <si>
     <t>""
 ""</t>
+  </si>
+  <si>
+    <t>1. Enter valid credentials 
+2. Click Login</t>
+  </si>
+  <si>
+    <t>User redirected to dashboard page</t>
   </si>
 </sst>
 </file>
@@ -850,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,34 +889,34 @@
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
@@ -911,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -920,19 +939,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -946,7 +965,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
@@ -955,19 +974,19 @@
         <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
@@ -978,10 +997,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -990,19 +1009,19 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -1013,10 +1032,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
@@ -1025,19 +1044,19 @@
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
@@ -1047,7 +1066,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
@@ -1056,19 +1075,19 @@
         <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
@@ -1079,10 +1098,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
@@ -1091,19 +1110,19 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>3</v>
@@ -1113,7 +1132,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -1122,19 +1141,19 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>3</v>
@@ -1148,7 +1167,7 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -1157,19 +1176,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>3</v>
@@ -1202,263 +1221,298 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
@@ -1473,6 +1527,7 @@
     <hyperlink ref="J7" r:id="rId4" display="unkown@gmail.com_x000a_Password123" xr:uid="{8E9299D3-48E0-4C38-B73F-1B32DD1DAF75}"/>
     <hyperlink ref="J8" r:id="rId5" xr:uid="{06B734FC-2BFE-49EA-8A3D-643EA76C66E3}"/>
     <hyperlink ref="J9" r:id="rId6" display="user1@gmail.com_x000a_&quot;&quot;" xr:uid="{80DFB4DC-83B4-45F7-BB88-3569EF28A690}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{C01B17C2-E00A-4A0F-B111-E6F3C59B8C05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upload TESCT CASE authorization 1
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35785A2C-E4D8-4305-A047-5EC2F588F24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB933406-196C-4369-9E27-DE0682BF156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Test" sheetId="1" r:id="rId1"/>
     <sheet name="Login Test" sheetId="8" r:id="rId2"/>
+    <sheet name="Authorization Module" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="121">
   <si>
     <t>Module</t>
   </si>
@@ -392,6 +393,35 @@
   </si>
   <si>
     <t>User redirected to dashboard page</t>
+  </si>
+  <si>
+    <t>AUTH-TC-01</t>
+  </si>
+  <si>
+    <t>AUTH-TS-01</t>
+  </si>
+  <si>
+    <t>AUTH-01</t>
+  </si>
+  <si>
+    <t>Authorization Module</t>
+  </si>
+  <si>
+    <t>Access restricted page without login</t>
+  </si>
+  <si>
+    <t>User not logged in</t>
+  </si>
+  <si>
+    <t>1. Open browser 
+2. Enter restricted page URL 
+3. Press Enter</t>
+  </si>
+  <si>
+    <t>Direct restricted URL</t>
+  </si>
+  <si>
+    <t>User cannot access restricted page</t>
   </si>
 </sst>
 </file>
@@ -514,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +564,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,12 +582,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1028,10 +1059,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1063,8 +1094,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="63" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1094,10 +1125,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1129,8 +1160,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="2" t="s">
         <v>64</v>
       </c>
@@ -1221,22 +1252,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1381,10 +1412,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1416,8 +1447,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="2" t="s">
         <v>101</v>
       </c>
@@ -1447,8 +1478,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="2" t="s">
         <v>105</v>
       </c>
@@ -1531,4 +1562,103 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63314DAE-2406-4F5E-8077-A60FAFEC120D}">
+  <dimension ref="C3:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="10.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload TESCT CASE authorization 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E78188-B79E-4511-A7D5-475AF79238B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F62D4-C232-4F4C-B1E6-E1F4026771B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="129">
   <si>
     <t>Module</t>
   </si>
@@ -425,6 +425,31 @@
   </si>
   <si>
     <t>Verify user cannot access restricted page without login</t>
+  </si>
+  <si>
+    <t>AUTH-02</t>
+  </si>
+  <si>
+    <t>AUTH-TC-02</t>
+  </si>
+  <si>
+    <t>AUTH-TS-02</t>
+  </si>
+  <si>
+    <t>Verify redirect to login when accessing
+ restricted page via direct URL</t>
+  </si>
+  <si>
+    <t>Access restricted page via direct 
+URL without login</t>
+  </si>
+  <si>
+    <t>1. Copy restricted page URL 
+2. Paste into browser 
+3. Press Enter</t>
+  </si>
+  <si>
+    <t>User redirected to login page</t>
   </si>
 </sst>
 </file>
@@ -547,7 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -586,6 +611,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1569,17 +1597,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63314DAE-2406-4F5E-8077-A60FAFEC120D}">
-  <dimension ref="C3:M4"/>
+  <dimension ref="C3:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="13"/>
     <col min="3" max="3" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
@@ -1661,7 +1689,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload TESCT CASE authorization 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F62D4-C232-4F4C-B1E6-E1F4026771B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95060F1E-BDB5-4BEF-AFFF-8CD878889BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="137">
   <si>
     <t>Module</t>
   </si>
@@ -450,6 +450,31 @@
   </si>
   <si>
     <t>User redirected to login page</t>
+  </si>
+  <si>
+    <t>AUTH-03</t>
+  </si>
+  <si>
+    <t>AUTH-TC-03</t>
+  </si>
+  <si>
+    <t>AUTH-TS-03</t>
+  </si>
+  <si>
+    <t>Verify logged-in user can access restricted page</t>
+  </si>
+  <si>
+    <t>Access restricted page after login</t>
+  </si>
+  <si>
+    <t>User logged in</t>
+  </si>
+  <si>
+    <t>1. Login with valid credentials 
+2. Navigate to restricted page</t>
+  </si>
+  <si>
+    <t>Restricted page successfully displayed</t>
   </si>
 </sst>
 </file>
@@ -1597,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63314DAE-2406-4F5E-8077-A60FAFEC120D}">
-  <dimension ref="C3:M5"/>
+  <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1639,7 @@
     <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="13"/>
   </cols>
@@ -1724,8 +1749,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{732FC934-1B67-4539-806A-28798A7C7EE3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE logout 1
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95060F1E-BDB5-4BEF-AFFF-8CD878889BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374CCD59-99B5-45DA-B2AC-065994591668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Test" sheetId="1" r:id="rId1"/>
     <sheet name="Login Test" sheetId="8" r:id="rId2"/>
-    <sheet name="Authorization Module" sheetId="9" r:id="rId3"/>
+    <sheet name="Authorization Test" sheetId="9" r:id="rId3"/>
+    <sheet name="Logout Test" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
   <si>
     <t>Module</t>
   </si>
@@ -475,6 +476,38 @@
   </si>
   <si>
     <t>Restricted page successfully displayed</t>
+  </si>
+  <si>
+    <t>LOGOUT-01</t>
+  </si>
+  <si>
+    <t>LOGOUT-TC-01</t>
+  </si>
+  <si>
+    <t>LOGOUT-TS-01</t>
+  </si>
+  <si>
+    <t>Verify user can logout successfully</t>
+  </si>
+  <si>
+    <t>Logout Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout after successful login </t>
+  </si>
+  <si>
+    <t>User already logged in</t>
+  </si>
+  <si>
+    <t>1. Click Logout button 
+2. Observe system response</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>User successfully logged out and 
+redirected to login/home page</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63314DAE-2406-4F5E-8077-A60FAFEC120D}">
   <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1791,4 +1824,103 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7880856C-9918-47AE-841F-8B6969F6EE15}">
+  <dimension ref="C3:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE logout 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374CCD59-99B5-45DA-B2AC-065994591668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873E730D-0407-4F98-BC00-D25208EBDE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="155">
   <si>
     <t>Module</t>
   </si>
@@ -508,6 +508,32 @@
   <si>
     <t>User successfully logged out and 
 redirected to login/home page</t>
+  </si>
+  <si>
+    <t>LOGOUT-02</t>
+  </si>
+  <si>
+    <t>LOGOUT-TC-02</t>
+  </si>
+  <si>
+    <t>LOGOUT-TS-02</t>
+  </si>
+  <si>
+    <t>Verify user cannot access restricted page after logout</t>
+  </si>
+  <si>
+    <t>Access resticted page after logout</t>
+  </si>
+  <si>
+    <t>User already logged out</t>
+  </si>
+  <si>
+    <t>1. Logout 
+2. Enter restricted page URL in browser 
+3. Press Enter</t>
+  </si>
+  <si>
+    <t>Directed restricted URL</t>
   </si>
 </sst>
 </file>
@@ -1828,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7880856C-9918-47AE-841F-8B6969F6EE15}">
-  <dimension ref="C3:M4"/>
+  <dimension ref="C3:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1870,7 @@
     <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="13"/>
@@ -1920,7 +1946,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE logout 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873E730D-0407-4F98-BC00-D25208EBDE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD280CA-FD98-408F-A1AC-E1B00042A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="163">
   <si>
     <t>Module</t>
   </si>
@@ -534,6 +534,32 @@
   </si>
   <si>
     <t>Directed restricted URL</t>
+  </si>
+  <si>
+    <t>LOGOUT-03</t>
+  </si>
+  <si>
+    <t>LOGOUT-TC-03</t>
+  </si>
+  <si>
+    <t>LOGOUT-TS-03</t>
+  </si>
+  <si>
+    <t>Verify user session is terminated after logout</t>
+  </si>
+  <si>
+    <t>Verify session is invalid after logout</t>
+  </si>
+  <si>
+    <t>User has logged in and then logged out</t>
+  </si>
+  <si>
+    <t>1. Logout 
+2. Refresh browser 
+3. Try to navigate to restricted page</t>
+  </si>
+  <si>
+    <t>Session is terminated and user is redirected to login page</t>
   </si>
 </sst>
 </file>
@@ -1854,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7880856C-9918-47AE-841F-8B6969F6EE15}">
-  <dimension ref="C3:M5"/>
+  <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1894,8 @@
     <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
@@ -1981,6 +2008,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upload TEST CASE Session 1
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD280CA-FD98-408F-A1AC-E1B00042A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC04E6-1F9B-43DF-93B9-BF0ECBC34E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Test" sheetId="1" r:id="rId1"/>
     <sheet name="Login Test" sheetId="8" r:id="rId2"/>
     <sheet name="Authorization Test" sheetId="9" r:id="rId3"/>
     <sheet name="Logout Test" sheetId="10" r:id="rId4"/>
+    <sheet name="Session Test" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="175">
   <si>
     <t>Module</t>
   </si>
@@ -560,6 +561,46 @@
   </si>
   <si>
     <t>Session is terminated and user is redirected to login page</t>
+  </si>
+  <si>
+    <t>SES-01</t>
+  </si>
+  <si>
+    <t>SES-02</t>
+  </si>
+  <si>
+    <t>SES-03</t>
+  </si>
+  <si>
+    <t>SES-TC-01</t>
+  </si>
+  <si>
+    <t>SES-TS-01</t>
+  </si>
+  <si>
+    <t>Verify session is active after successful login</t>
+  </si>
+  <si>
+    <t>Session Module</t>
+  </si>
+  <si>
+    <t>Verify session is created after 
+successful login</t>
+  </si>
+  <si>
+    <t>User has valid account</t>
+  </si>
+  <si>
+    <t>1. Open login page 
+2. Enter valid email and password 
+3. Click Login 
+4. Access restricted page</t>
+  </si>
+  <si>
+    <t>Valid email &amp; password</t>
+  </si>
+  <si>
+    <t>User successfully logged in and can access restricted pages without re-login</t>
   </si>
 </sst>
 </file>
@@ -1882,7 +1923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7880856C-9918-47AE-841F-8B6969F6EE15}">
   <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -2047,4 +2088,175 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B621CD39-D3B1-47CB-8E0E-3CB76FE47CFC}">
+  <dimension ref="C3:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE Session 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC04E6-1F9B-43DF-93B9-BF0ECBC34E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E11761-699F-4F4E-874D-2B7987940DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="181">
   <si>
     <t>Module</t>
   </si>
@@ -601,6 +601,26 @@
   </si>
   <si>
     <t>User successfully logged in and can access restricted pages without re-login</t>
+  </si>
+  <si>
+    <t>SES-TC-02</t>
+  </si>
+  <si>
+    <t>SES-TS-02</t>
+  </si>
+  <si>
+    <t>Verify session is terminated after logout</t>
+  </si>
+  <si>
+    <t>Verify session is destroyed after logout</t>
+  </si>
+  <si>
+    <t>1. Click Logout 
+2. Try to refresh page 
+3. Try to access restricted page</t>
+  </si>
+  <si>
+    <t>Session is invalidated and user is redirected to login page</t>
   </si>
 </sst>
 </file>
@@ -2095,7 +2115,7 @@
   <dimension ref="C3:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2106,8 +2126,7 @@
     <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32" style="13" bestFit="1" customWidth="1"/>
@@ -2185,36 +2204,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>164</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
upload TEST CASE Session 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E11761-699F-4F4E-874D-2B7987940DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A065D7-0209-4564-8F91-EC4F6C1EF063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
   <si>
     <t>Module</t>
   </si>
@@ -621,6 +621,29 @@
   </si>
   <si>
     <t>Session is invalidated and user is redirected to login page</t>
+  </si>
+  <si>
+    <t>SES-TC-03</t>
+  </si>
+  <si>
+    <t>SES-TS-03</t>
+  </si>
+  <si>
+    <t>Verify restricted page cannot be accessed 
+using browser back button after logout</t>
+  </si>
+  <si>
+    <t>Verify restricted page cannot be accessed 
+via browser back after logout</t>
+  </si>
+  <si>
+    <t>1. Login 
+2. Access restricted page 
+3. Logout 
+4. Click browser Back button</t>
+  </si>
+  <si>
+    <t>System prevents access and redirects user to login page</t>
   </si>
 </sst>
 </file>
@@ -2115,7 +2138,7 @@
   <dimension ref="C3:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2243,32 +2266,32 @@
       <c r="C6" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>158</v>
+      <c r="D6" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>159</v>
+        <v>182</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>160</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>145</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
upload TEST CASE UI 1
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A065D7-0209-4564-8F91-EC4F6C1EF063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CD44F5-8D4D-45B5-9E92-611AAAEC27D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Test" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Authorization Test" sheetId="9" r:id="rId3"/>
     <sheet name="Logout Test" sheetId="10" r:id="rId4"/>
     <sheet name="Session Test" sheetId="11" r:id="rId5"/>
+    <sheet name="UI Test" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="197">
   <si>
     <t>Module</t>
   </si>
@@ -644,6 +645,37 @@
   </si>
   <si>
     <t>System prevents access and redirects user to login page</t>
+  </si>
+  <si>
+    <t>UI-01</t>
+  </si>
+  <si>
+    <t>UI-TC-01</t>
+  </si>
+  <si>
+    <t>UI-TS-01</t>
+  </si>
+  <si>
+    <t>UI Module</t>
+  </si>
+  <si>
+    <t>Verify error message is clearly visible to the user</t>
+  </si>
+  <si>
+    <t>Verify error message visibility</t>
+  </si>
+  <si>
+    <t>User is on login or registration page</t>
+  </si>
+  <si>
+    <t>1. Submit form with invalid data 
+2. Observe displayed error message</t>
+  </si>
+  <si>
+    <t>Invalid email/password</t>
+  </si>
+  <si>
+    <t>Error message is clearly visible, readable, and positioned near related field</t>
   </si>
 </sst>
 </file>
@@ -2137,7 +2169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B621CD39-D3B1-47CB-8E0E-3CB76FE47CFC}">
   <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -2301,4 +2333,173 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E0D66A-A962-4F7B-A455-3BF4CEA431B5}">
+  <dimension ref="C3:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE UI 2
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CD44F5-8D4D-45B5-9E92-611AAAEC27D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F962812-E593-4AB4-9632-991296D0F64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="205">
   <si>
     <t>Module</t>
   </si>
@@ -676,6 +676,34 @@
   </si>
   <si>
     <t>Error message is clearly visible, readable, and positioned near related field</t>
+  </si>
+  <si>
+    <t>UI-02</t>
+  </si>
+  <si>
+    <t>UI-TC-02</t>
+  </si>
+  <si>
+    <t>UI-TS-02</t>
+  </si>
+  <si>
+    <t>Verify form validation appears when input is incorrect</t>
+  </si>
+  <si>
+    <t>User is on form page</t>
+  </si>
+  <si>
+    <t>Verify validation message for
+ incorrect input</t>
+  </si>
+  <si>
+    <t>1. Enter invalid email format 
+2. Leave required field empty 
+3. Click Submit</t>
+  </si>
+  <si>
+    <t>Invalid email format, 
+empty required field</t>
   </si>
 </sst>
 </file>
@@ -2340,7 +2368,7 @@
   <dimension ref="C3:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2431,31 +2459,31 @@
     </row>
     <row r="5" spans="3:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>178</v>
+        <v>199</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>143</v>
+        <v>201</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>145</v>
+        <v>203</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>180</v>
@@ -2500,6 +2528,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload TEST CASE UI 3
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F962812-E593-4AB4-9632-991296D0F64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B0EB3-62EB-4BE3-9C02-5627DB82661B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
   <si>
     <t>Module</t>
   </si>
@@ -704,6 +704,38 @@
   <si>
     <t>Invalid email format, 
 empty required field</t>
+  </si>
+  <si>
+    <t>Validation message appears for each incorrect field</t>
+  </si>
+  <si>
+    <t>UI-03</t>
+  </si>
+  <si>
+    <t>UI-TC-03</t>
+  </si>
+  <si>
+    <t>Verify system display is responsive on mobile devices</t>
+  </si>
+  <si>
+    <t>UI-TS-03</t>
+  </si>
+  <si>
+    <t>Verify system responsiveness on mobile view</t>
+  </si>
+  <si>
+    <t>Application is accessible</t>
+  </si>
+  <si>
+    <t>1. Open application in browser 
+2. Switch to mobile view (responsive mode) 
+3. Navigate through pages</t>
+  </si>
+  <si>
+    <t>Mobile screen resolution</t>
+  </si>
+  <si>
+    <t>Layout adjusts properly, no overlapping text/buttons, all features accessible</t>
   </si>
 </sst>
 </file>
@@ -2367,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E0D66A-A962-4F7B-A455-3BF4CEA431B5}">
   <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2486,7 +2518,7 @@
         <v>204</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>3</v>
@@ -2494,34 +2526,34 @@
     </row>
     <row r="6" spans="3:13" ht="63" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>145</v>
+        <v>213</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
update TEST CASE login
</commit_message>
<xml_diff>
--- a/documentation/TEST CASE.xlsx
+++ b/documentation/TEST CASE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worpdress Blog Manual Testing\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076B0EB3-62EB-4BE3-9C02-5627DB82661B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942C79AE-0FF6-4A04-A729-19F8418B1866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="5" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{99208258-F126-4562-88E1-3DA1320E1714}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration Test" sheetId="1" r:id="rId1"/>
@@ -878,11 +878,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -896,9 +894,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1217,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A25FA9-3B9D-44C9-86EA-75B357B6CC75}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91A25A-752B-4207-94CE-F7CCA5E95DB5}">
   <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,10 +1729,10 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1764,8 +1764,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
         <v>101</v>
       </c>
@@ -1795,8 +1795,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
         <v>105</v>
       </c>
@@ -1891,18 +1891,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13"/>
-    <col min="3" max="3" width="10.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="33" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="33" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
       <c r="C5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="8" t="s">
         <v>125</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -2014,7 +2014,7 @@
       <c r="C6" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>132</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -2064,19 +2064,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13"/>
-    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
@@ -2235,18 +2235,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13"/>
-    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
       <c r="C6" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -2399,24 +2399,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E0D66A-A962-4F7B-A455-3BF4CEA431B5}">
   <dimension ref="C3:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="13"/>
-    <col min="3" max="3" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="35.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
@@ -2528,7 +2528,7 @@
       <c r="C6" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>208</v>
       </c>
       <c r="E6" s="2" t="s">

</xml_diff>